<commit_message>
add first microservice, and test call by angular web
</commit_message>
<xml_diff>
--- a/Design&Spec/Design.xlsx
+++ b/Design&Spec/Design.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1A71F0-1246-4C52-BC61-7371838B8EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EC013F-B442-4E4C-8FC2-1C99C871AAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="4590" windowWidth="21600" windowHeight="11820" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FunctionOverview" sheetId="1" r:id="rId1"/>
@@ -3567,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AK134"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7800,9 +7800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2966A73-4336-46F7-A49C-4EE5560BE154}">
   <dimension ref="B2:BP79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AY28" sqref="AY28"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12806,9 +12804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D214BE-E37F-4573-86FC-E2A12F63C0AA}">
   <dimension ref="B2:BP138"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M110" sqref="M106:M110"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21690,7 +21686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399ACCA1-7C19-4771-8440-355B030FBAEA}">
   <dimension ref="B2:BP92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -26830,7 +26826,7 @@
   <dimension ref="B2:BP21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -28255,7 +28251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841EB371-A22F-4155-BB19-6225587F06A6}">
   <dimension ref="B2:AH40"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29605,9 +29601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232E16C2-B7D9-4899-AFA9-6D2E8ABCB180}">
   <dimension ref="B2:AH60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z55" sqref="Z55"/>
-    </sheetView>
+    <sheetView showGridLines="0" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>